<commit_message>
Alpha shadow build 0.1.1 Add missed points
</commit_message>
<xml_diff>
--- a/configPoints.xlsx
+++ b/configPoints.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73439AE-AF48-450E-A635-EF42559F5957}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE7ABD8-EA43-4A3D-A15C-F9C88F5CB386}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="497">
   <si>
     <t>Номер помещения</t>
   </si>
@@ -1484,6 +1484,54 @@
   </si>
   <si>
     <t>334D</t>
+  </si>
+  <si>
+    <t>PKR</t>
+  </si>
+  <si>
+    <t>exitP</t>
+  </si>
+  <si>
+    <t>AnP</t>
+  </si>
+  <si>
+    <t>List Shafls</t>
+  </si>
+  <si>
+    <t>An</t>
+  </si>
+  <si>
+    <t>2.13</t>
+  </si>
+  <si>
+    <t>53D</t>
+  </si>
+  <si>
+    <t>2.12</t>
+  </si>
+  <si>
+    <t>56D</t>
+  </si>
+  <si>
+    <t>55D</t>
+  </si>
+  <si>
+    <t>2.14.1</t>
+  </si>
+  <si>
+    <t>58D</t>
+  </si>
+  <si>
+    <t>57D</t>
+  </si>
+  <si>
+    <t>54D</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>140D</t>
   </si>
 </sst>
 </file>
@@ -2027,7 +2075,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D24"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2375,11 +2423,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99587236-7E1B-4FF4-9D1D-9EFAAE802114}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D18"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2528,13 +2576,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>374</v>
+        <v>486</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>375</v>
+        <v>487</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -2542,13 +2590,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>374</v>
+        <v>488</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>376</v>
+        <v>489</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
@@ -2556,13 +2604,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>377</v>
+        <v>488</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>378</v>
+        <v>490</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
@@ -2570,13 +2618,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>377</v>
+        <v>491</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>379</v>
+        <v>492</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
@@ -2584,48 +2632,132 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>380</v>
+        <v>491</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>381</v>
+        <v>493</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
+        <v>214</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>215</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>216</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>217</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>218</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>222</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
         <v>233</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="12"/>
+      <c r="D24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2644,7 +2776,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D18"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2915,7 +3047,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D33"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4147,7 +4279,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4375,6 +4507,20 @@
         <v>480</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>514</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4594,11 +4740,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87333CA0-39BE-4E21-97E2-7A7B7331CECB}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D36"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4648,56 +4794,56 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>100</v>
+      <c r="A5" s="12">
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>481</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>101</v>
+      <c r="A6" s="12">
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>482</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>102</v>
+      <c r="A7" s="12">
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>483</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>103</v>
+      <c r="A8" s="12">
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>484</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>485</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>
@@ -4705,13 +4851,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
@@ -4719,13 +4865,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>26</v>
@@ -4733,13 +4879,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>26</v>
@@ -4747,13 +4893,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>26</v>
@@ -4761,13 +4907,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>26</v>
@@ -4775,13 +4921,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>26</v>
@@ -4789,13 +4935,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>26</v>
@@ -4803,13 +4949,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>26</v>
@@ -4817,13 +4963,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>26</v>
@@ -4831,13 +4977,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
@@ -4845,13 +4991,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>26</v>
@@ -4859,13 +5005,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>26</v>
@@ -4873,13 +5019,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>26</v>
@@ -4887,13 +5033,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>26</v>
@@ -4901,13 +5047,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>26</v>
@@ -4915,13 +5061,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>26</v>
@@ -4929,13 +5075,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>26</v>
@@ -4943,13 +5089,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>26</v>
@@ -4957,13 +5103,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>26</v>
@@ -4971,13 +5117,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>26</v>
@@ -4985,13 +5131,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>26</v>
@@ -4999,13 +5145,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>26</v>
@@ -5013,13 +5159,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>26</v>
@@ -5027,13 +5173,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>26</v>
@@ -5041,13 +5187,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>272</v>
+        <v>108</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>26</v>
@@ -5055,13 +5201,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>272</v>
+        <v>110</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>26</v>
@@ -5069,13 +5215,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>272</v>
+        <v>112</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>26</v>
@@ -5083,21 +5229,77 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
+        <v>128</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>129</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>130</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>131</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
         <v>132</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A5:D36">
-    <sortCondition ref="A5"/>
+  <sortState ref="A9:D40">
+    <sortCondition ref="A9"/>
   </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{ED561688-7D7A-4D49-9280-148E5D6726B9}">
@@ -5114,7 +5316,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -6261,7 +6463,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D23"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6942,7 +7144,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D24"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Alpha shadow build 0.1.4.t1 Add Group Sun Time
</commit_message>
<xml_diff>
--- a/configPoints.xlsx
+++ b/configPoints.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC77B3AB-FF3E-4138-B87A-D40B9512FADF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C657FF-B72D-47B5-92A5-686143408A58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DESCRIPTION" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="495">
   <si>
     <t>Номер помещения</t>
   </si>
@@ -1520,6 +1520,12 @@
   </si>
   <si>
     <t>Controller Register:</t>
+  </si>
+  <si>
+    <t>Sun Time</t>
+  </si>
+  <si>
+    <t>outdoor</t>
   </si>
 </sst>
 </file>
@@ -2487,7 +2493,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5134,7 +5140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87333CA0-39BE-4E21-97E2-7A7B7331CECB}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
@@ -7123,11 +7129,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F009337-4AB3-4E3F-9EC9-9C14447D700E}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7188,48 +7194,48 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>175</v>
+      <c r="A6" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>285</v>
+        <v>493</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>321</v>
+        <v>494</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="9">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>272</v>
+        <v>321</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="9">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>64</v>
+        <v>272</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>
@@ -7240,13 +7246,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>275</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
@@ -7257,13 +7263,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>275</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>26</v>
@@ -7274,13 +7280,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>26</v>
@@ -7291,13 +7297,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>279</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>26</v>
@@ -7308,13 +7314,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>26</v>
@@ -7325,13 +7331,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>281</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>26</v>
@@ -7342,13 +7348,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>284</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>26</v>
@@ -7359,13 +7365,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>26</v>
@@ -7376,13 +7382,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>285</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>26</v>
@@ -7393,13 +7399,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>285</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>81</v>
+        <v>287</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
@@ -7410,13 +7416,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>26</v>
@@ -7427,13 +7433,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>290</v>
+        <v>137</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>26</v>
@@ -7444,18 +7450,35 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
+        <v>189</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
         <v>190</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="9">
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>